<commit_message>
SWRS_BRMTR_006 added to the requirements.
</commit_message>
<xml_diff>
--- a/code_borimeter/Documentation/swrs_borimeter.xlsx
+++ b/code_borimeter/Documentation/swrs_borimeter.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\users\F10553C\Documents\Git Repo\borimeter\docu_borimeter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\users\F10553C\Documents\Git Repo\borimeter\code_borimeter\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>SWRS_BRMTR_001</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>A unique ID shall be calculated for each user, based on their personal information.</t>
+  </si>
+  <si>
+    <t>SWRS_BRMTR_006</t>
+  </si>
+  <si>
+    <t>Images shall be displayed for 500ms. After this they should disappear, and a grey backround shall be visible.</t>
   </si>
 </sst>
 </file>
@@ -161,17 +167,23 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color rgb="FF595959"/>
+        <color rgb="FF262626"/>
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
       <fill>
-        <patternFill patternType="none">
+        <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor rgb="FFF2F2F2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -192,6 +204,36 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF262626"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -215,7 +257,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -259,53 +301,17 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color rgb="FF262626"/>
+        <color rgb="FF595959"/>
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
+        <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFF2F2F2"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF262626"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -721,14 +727,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="wishlist" displayName="wishlist" ref="B2:E9" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" totalsRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="wishlist" displayName="wishlist" ref="B2:E10" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" totalsRowDxfId="8">
   <tableColumns count="4">
     <tableColumn id="1" name="Requirement ID" dataDxfId="7" totalsRowDxfId="6">
       <calculatedColumnFormula>ROW()-2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Requirement Specification" dataDxfId="2" totalsRowDxfId="5"/>
-    <tableColumn id="3" name="Type" dataDxfId="0" totalsRowDxfId="3"/>
-    <tableColumn id="2" name="Status" dataDxfId="1" totalsRowDxfId="4"/>
+    <tableColumn id="7" name="Requirement Specification" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="3" name="Type" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="2" name="Status" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Oszkar List Style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1000,10 +1006,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="B2:E9"/>
+  <dimension ref="B2:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1127,6 +1133,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="10" spans="2:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>